<commit_message>
Updates to DA and Lexicon
</commit_message>
<xml_diff>
--- a/Dzaqtlas Adventures Chapters/Assets/Tables.xlsx
+++ b/Dzaqtlas Adventures Chapters/Assets/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffkazmierski/Documents/GitHub/Zdetl/Dzaqtlas Adventures Chapters/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AF19BD-72AF-BC46-9380-339D87F068FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13305E67-A2EF-7649-8A9A-2A9C4032B298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15880" activeTab="3" xr2:uid="{68ED0E21-30F5-114A-A1AB-58F817155603}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15880" activeTab="4" xr2:uid="{68ED0E21-30F5-114A-A1AB-58F817155603}"/>
   </bookViews>
   <sheets>
     <sheet name="Zhodani Life Events" sheetId="1" r:id="rId1"/>
@@ -2392,8 +2392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7231114-CFEC-014D-910B-67D467BB9B85}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2564,6 +2564,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2571,8 +2572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129FA5D8-DEE4-A741-B49E-288412A0AA82}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates to CZ files
</commit_message>
<xml_diff>
--- a/Dzaqtlas Adventures Chapters/Assets/Tables.xlsx
+++ b/Dzaqtlas Adventures Chapters/Assets/Tables.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffkazmierski/Documents/GitHub/Zdetl/Dzaqtlas Adventures Chapters/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13305E67-A2EF-7649-8A9A-2A9C4032B298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E390DC-7573-7149-A8E7-FF75FDB8F028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15880" activeTab="4" xr2:uid="{68ED0E21-30F5-114A-A1AB-58F817155603}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{68ED0E21-30F5-114A-A1AB-58F817155603}"/>
   </bookViews>
   <sheets>
-    <sheet name="Zhodani Life Events" sheetId="1" r:id="rId1"/>
-    <sheet name="Agent Life Events" sheetId="2" r:id="rId2"/>
-    <sheet name="Army Tables" sheetId="3" r:id="rId3"/>
-    <sheet name="Aviator Tables" sheetId="13" r:id="rId4"/>
-    <sheet name="Citizen Life Events" sheetId="11" r:id="rId5"/>
-    <sheet name="Drifter Life Events" sheetId="4" r:id="rId6"/>
-    <sheet name="Entertainer Life Events" sheetId="5" r:id="rId7"/>
-    <sheet name="Government Life Events" sheetId="6" r:id="rId8"/>
-    <sheet name="Merchant Life Events" sheetId="7" r:id="rId9"/>
-    <sheet name="Navy Life Events" sheetId="8" r:id="rId10"/>
-    <sheet name="Nobility Life Events" sheetId="12" r:id="rId11"/>
-    <sheet name="Rogue Life Events" sheetId="10" r:id="rId12"/>
-    <sheet name="Scholar Life Events" sheetId="9" r:id="rId13"/>
+    <sheet name="Wasteland Timeline" sheetId="15" r:id="rId1"/>
+    <sheet name="End of Days Timeline" sheetId="14" r:id="rId2"/>
+    <sheet name="Zhodani Life Events" sheetId="1" r:id="rId3"/>
+    <sheet name="Agent Life Events" sheetId="2" r:id="rId4"/>
+    <sheet name="Army Tables" sheetId="3" r:id="rId5"/>
+    <sheet name="Aviator Tables" sheetId="13" r:id="rId6"/>
+    <sheet name="Citizen Life Events" sheetId="11" r:id="rId7"/>
+    <sheet name="Drifter Life Events" sheetId="4" r:id="rId8"/>
+    <sheet name="Entertainer Life Events" sheetId="5" r:id="rId9"/>
+    <sheet name="Government Life Events" sheetId="6" r:id="rId10"/>
+    <sheet name="Merchant Life Events" sheetId="7" r:id="rId11"/>
+    <sheet name="Navy Life Events" sheetId="8" r:id="rId12"/>
+    <sheet name="Nobility Life Events" sheetId="12" r:id="rId13"/>
+    <sheet name="Rogue Life Events" sheetId="10" r:id="rId14"/>
+    <sheet name="Scholar Life Events" sheetId="9" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="93">
   <si>
     <t>Life Events</t>
   </si>
@@ -819,12 +821,60 @@
       <t>You make a Contact outside your normal circles.</t>
     </r>
   </si>
+  <si>
+    <t>Teqozdij</t>
+  </si>
+  <si>
+    <t>First space exploration</t>
+  </si>
+  <si>
+    <t>First expedition to Viepchakl</t>
+  </si>
+  <si>
+    <t>Second Dark Age begins.</t>
+  </si>
+  <si>
+    <t>Power grids begin to fail as the crews die and monitoring ceases.</t>
+  </si>
+  <si>
+    <t>Terrestrial agriculture begins to fail,  food distribution collapses.</t>
+  </si>
+  <si>
+    <t>Food riots as famine deepens. Survivors flee cities.</t>
+  </si>
+  <si>
+    <t>Campaign begins.</t>
+  </si>
+  <si>
+    <t>Viepchakl base established. First contact between Zhodani humans and Viepchaklts chirpers</t>
+  </si>
+  <si>
+    <t>First Qiknavrats-Viepchaklts meetings. Dzaqtlas begins.</t>
+  </si>
+  <si>
+    <t>Qiknavrats extinction. Dzaqtlas spreads to Zhdant.</t>
+  </si>
+  <si>
+    <t>Viepchaklts extinction. Medical infrastructure collapses. Dzaqtlas at its height. Plague rages unchecked, reaching 40% mortality.</t>
+  </si>
+  <si>
+    <t>Water and food production becomes a transmission vector. Famine exacerbates the effect of the plague, mortality 60%.</t>
+  </si>
+  <si>
+    <t>Survivalist communities form. Mobile gangs terrorize the wasteland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight from cities. Power grids begin to fail. </t>
+  </si>
+  <si>
+    <t>Collapse of coastal cities. Without maintenance, buildings succumb to corrosion and weathering.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -844,6 +894,19 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -866,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -885,6 +948,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,6 +1283,1057 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA9F809-CDAE-CE48-BA4E-8D50ADD3A263}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="87.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-530</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-510</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-350</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2384AD8-7B5F-9F4D-B9A4-8A17115238CE}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8B5108-43EE-B141-96CF-87AC8570C4FF}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7DDEE4-9EA1-924D-A9FB-26B48B4ABD66}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577BEB27-294E-AD4D-BE84-D994AEC57031}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94740D35-DA0A-384E-819F-C2241B567235}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85A8A1B-65C7-024C-9BE9-D269DE3F4D35}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D482FA-44C3-CF47-8133-A755F6DEB82F}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView zoomScale="134" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="106.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>-549.1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>-539.29999999999995</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>-535.29999999999995</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>-535.20000000000005</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>-534.29999999999995</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>-533.20000000000005</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>-533.1</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>-532.29999999999995</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>-532.20000000000005</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>-531.29999999999995</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>-531.20000000000005</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>-531.1</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F30F66-C22F-ED48-8033-402DE6EF0263}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -1341,579 +2457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7DDEE4-9EA1-924D-A9FB-26B48B4ABD66}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577BEB27-294E-AD4D-BE84-D994AEC57031}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94740D35-DA0A-384E-819F-C2241B567235}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85A8A1B-65C7-024C-9BE9-D269DE3F4D35}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FF617E-B240-EC49-A224-583F89EE7160}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -2092,7 +2636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB59521-647D-8B42-AE41-14953BF187FA}">
   <dimension ref="A1:F21"/>
   <sheetViews>
@@ -2388,7 +2932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7231114-CFEC-014D-910B-67D467BB9B85}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -2568,11 +3112,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129FA5D8-DEE4-A741-B49E-288412A0AA82}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2712,7 +3256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119C641C-3468-B04D-B4CF-20907F9CA8BA}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -2855,7 +3399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF0771B-824A-A543-9945-94762B9CF323}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -2996,290 +3540,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2384AD8-7B5F-9F4D-B9A4-8A17115238CE}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8B5108-43EE-B141-96CF-87AC8570C4FF}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="77.33203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>